<commit_message>
added write back with ram still has a problem with switching banks. it seems to write and read from same bank
</commit_message>
<xml_diff>
--- a/Excel/CRC_CALC.xlsx
+++ b/Excel/CRC_CALC.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Type</t>
   </si>
@@ -36,10 +36,25 @@
     <t>CRC [hex]</t>
   </si>
   <si>
-    <t>Payload (1,2,3,4)</t>
-  </si>
-  <si>
-    <t>FF</t>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payload </t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>F6</t>
   </si>
 </sst>
 </file>
@@ -86,7 +101,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -104,7 +119,108 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
@@ -115,33 +231,47 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top/>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -445,102 +575,162 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F1:K6"/>
+  <dimension ref="L7:R20"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="10" max="10" width="2.875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.25" customWidth="1"/>
+    <col min="17" max="17" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="F1" s="3" t="s">
+    <row r="7" spans="12:18" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="12:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="M8" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-    </row>
-    <row r="2" spans="6:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="F2">
-        <f>HEX2DEC(J2)</f>
-        <v>128</v>
-      </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5">
-        <f>80</f>
-        <v>80</v>
-      </c>
-      <c r="K2" s="3" t="s">
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="4"/>
+    </row>
+    <row r="9" spans="12:18" ht="15" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <f>HEX2DEC(P9)</f>
+        <v>1</v>
+      </c>
+      <c r="M9" s="6"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="6:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="F3">
-        <f>HEX2DEC(J3)</f>
+    <row r="10" spans="12:18" ht="15" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <f>HEX2DEC(P10)</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="9"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="12:18" ht="15" x14ac:dyDescent="0.25">
+      <c r="L11">
+        <f>HEX2DEC(P11)</f>
+        <v>5</v>
+      </c>
+      <c r="M11" s="9"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="10">
+        <v>5</v>
+      </c>
+      <c r="Q11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5">
-        <v>2</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="6:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="F4">
-        <f>HEX2DEC(J4)</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5">
-        <v>0</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F5" s="1">
-        <f>HEX2DEC(I5)+HEX2DEC(H5)+HEX2DEC(J5)+HEX2DEC(G5)</f>
-        <v>255</v>
-      </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1" t="s">
+    </row>
+    <row r="12" spans="12:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L12" s="1">
+        <f>SUM((Q15:Q24))</f>
+        <v>1221</v>
+      </c>
+      <c r="M12" s="11"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="12"/>
+    </row>
+    <row r="13" spans="12:18" ht="18" x14ac:dyDescent="0.25">
+      <c r="L13" s="2" t="str">
+        <f>DEC2HEX(MOD(SUM(L9:L11,L12),256))</f>
+        <v>CB</v>
+      </c>
+      <c r="M13" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q13" s="13"/>
+    </row>
+    <row r="14" spans="12:18" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q14" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="R14" s="17"/>
+    </row>
+    <row r="15" spans="12:18" x14ac:dyDescent="0.2">
+      <c r="Q15">
+        <f>HEX2DEC(R15)</f>
+        <v>161</v>
+      </c>
+      <c r="R15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="12:18" x14ac:dyDescent="0.2">
+      <c r="Q16">
+        <f>HEX2DEC(R16)</f>
+        <v>178</v>
+      </c>
+      <c r="R16" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="6:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="F6" s="2" t="str">
-        <f>DEC2HEX(MOD(SUM(F2:F4,F5),256))</f>
-        <v>81</v>
-      </c>
-      <c r="G6" t="s">
-        <v>5</v>
+    </row>
+    <row r="17" spans="17:18" x14ac:dyDescent="0.2">
+      <c r="Q17">
+        <f t="shared" ref="Q17:Q20" si="0">HEX2DEC(R17)</f>
+        <v>195</v>
+      </c>
+      <c r="R17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="17:18" x14ac:dyDescent="0.2">
+      <c r="Q18">
+        <f t="shared" si="0"/>
+        <v>212</v>
+      </c>
+      <c r="R18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="17:18" x14ac:dyDescent="0.2">
+      <c r="Q19">
+        <f t="shared" si="0"/>
+        <v>229</v>
+      </c>
+      <c r="R19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="17:18" x14ac:dyDescent="0.2">
+      <c r="Q20">
+        <f t="shared" si="0"/>
+        <v>246</v>
+      </c>
+      <c r="R20" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="G1:J1"/>
+  <mergeCells count="2">
+    <mergeCell ref="M8:P8"/>
+    <mergeCell ref="Q14:R14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>